<commit_message>
I hope you see the files updated, final try.
</commit_message>
<xml_diff>
--- a/Data Base Fields.xlsx
+++ b/Data Base Fields.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">LAB TESTS</t>
   </si>
@@ -71,6 +71,15 @@
   </si>
   <si>
     <t xml:space="preserve">INVASIVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOCTOR’S NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEDICAL LICENSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSTITUTE / HOSPITAL</t>
   </si>
 </sst>
 </file>
@@ -85,6 +94,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -149,7 +159,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -174,24 +184,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:O3"/>
+  <dimension ref="A2:R3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection pane="topLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="9.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="22.36"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -249,6 +263,15 @@
       </c>
       <c r="O3" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>